<commit_message>
CBLHJB05 IPO nearly complete.
</commit_message>
<xml_diff>
--- a/CBLHJB05/CBLHJB05 IPO.xlsx
+++ b/CBLHJB05/CBLHJB05 IPO.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAWI19\CBLHJB05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69586062-4BF6-48A3-976D-BE587E458502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B47E5EC-3558-4788-8B95-F12B87B4F035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10455" yWindow="1695" windowWidth="15375" windowHeight="7875" xr2:uid="{C44F7549-E86D-4E3B-B41E-4CA174E0BEEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C44F7549-E86D-4E3B-B41E-4CA174E0BEEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="VAL_POP_TYPE">Sheet1!$H$3:$H$8</definedName>
+    <definedName name="VAL_STATES">Sheet1!$E$3:$E$8</definedName>
+    <definedName name="VAL_TEAM">Sheet1!$J$3:$J$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>I-LNAME</t>
   </si>
@@ -153,13 +180,55 @@
   </si>
   <si>
     <t>ERR-SW</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>NE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +236,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -256,13 +337,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -271,23 +359,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,20 +686,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3738D6A-8517-4BBC-BFB3-6E8A8C77C036}">
-  <dimension ref="A1:AJ20"/>
+  <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -627,59 +712,59 @@
     <col min="22" max="23" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="3" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="8" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ1" s="2"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="10"/>
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -712,217 +797,424 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AC2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AD2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AE2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AF2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AG2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AH2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AI2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="J3" s="1"/>
-      <c r="K3" s="10"/>
-      <c r="Y3" s="1"/>
-      <c r="AH3" s="1"/>
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="15">
+        <v>99999</v>
+      </c>
+      <c r="G3" s="15">
+        <v>9999</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>99</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" cm="1">
+        <f t="array" ref="L3">_xlfn.SWITCH(E3,"IA",0.05,"NE",0.05,"WI",0.05,"MI",0.1,"IL",0,"MO",0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="M3">
+        <f>L3 * (24 * I3)</f>
+        <v>118.80000000000001</v>
+      </c>
+      <c r="N3">
+        <f>(18.71 * I3) + M3</f>
+        <v>1971.0900000000001</v>
+      </c>
+      <c r="O3">
+        <f>IF(H3 = 1, I3,0)</f>
+        <v>99</v>
+      </c>
+      <c r="P3">
+        <f>IF(H3 = 2, I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>IF(H3 = 3, I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>IF(H3 = 4, I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>IF(H3 = 5, I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>IF(H3 = 6, I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>IF(J3 = "A", N3,0)</f>
+        <v>1971.0900000000001</v>
+      </c>
+      <c r="V3">
+        <f>IF(J3 = "B", N3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>IF(J3 = "C", N3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>IF(J3 = "D", N3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>IF(J3 = "E", N3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1" t="str" cm="1">
+        <f t="array" ref="AA3:AA8">IF(ISBLANK(A3),"LAST NAME REQUIRED",IF(ISBLANK(B3),"FIRST NAME REQUIRED",IF(ISBLANK(C3),"ADDRESS REQUIRED",IF(ISBLANK(D3),"CITY REQUIRED",IF(NOT(E3=VAL_STATES),"STATES MUST BE IA, IL, MI, MO, NE, OR WI",IF(NOT(ISNUMBER(_xlfn.CONCAT(F3,G3))),"ZIP CODE MUST BE NUMERIC",IF(ISNUMBER(H3),IF(H3=VAL_POP_TYPE,IF(ISNUMBER(I3),IF(I3&lt;1,"MINIMUM OF 1 CASE",IF(J3=VAL_TEAM,"","TEAM MUST BE A, B, C, D, OR E")),"POP TYPE MUST BE 1-6"),"POP TYPE MUST BE NUMERIC"))))))))</f>
+        <v>ZIP CODE MUST BE NUMERIC</v>
+      </c>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="J4" s="1"/>
-      <c r="K4" s="10"/>
-      <c r="Y4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="O4">
+        <f>IF(H4 = 1, O3+I4, O3)</f>
+        <v>99</v>
+      </c>
+      <c r="P4">
+        <f>IF(I4 = 2, P3+I4, P3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f>IF(J4 = 3, Q3+I4, Q3)</f>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>IF(K4 = 4, R3+I4, R3)</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f>IF(L4 = 5, S3+I4, S3)</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>IF(M4 = 6, T3+I4, T3)</f>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>IF(J4 = "A", U3+N4,U3)</f>
+        <v>1971.0900000000001</v>
+      </c>
+      <c r="V4">
+        <f>IF(J4 = "B", V3+N4,V3)</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>IF(J4 = "C", W3+N4,W3)</f>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f>IF(J4 = "D", X3+N4,X3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f>IF(J4 = "E", Y3+N4,Y3)</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="J5" s="1"/>
-      <c r="K5" s="10"/>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="14">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="5"/>
       <c r="Y5" s="1"/>
-      <c r="AH5" s="1"/>
+      <c r="AA5" s="1" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="AJ5" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="J6" s="1"/>
-      <c r="K6" s="10"/>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="14">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="5"/>
       <c r="Y6" s="1"/>
-      <c r="AH6" s="1"/>
+      <c r="AA6" s="1" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="AJ6" s="1"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="J7" s="1"/>
-      <c r="K7" s="10"/>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="14">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="5"/>
       <c r="Y7" s="1"/>
-      <c r="AH7" s="1"/>
+      <c r="AA7" s="1" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="14">
+        <v>6</v>
+      </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="10"/>
+      <c r="K8" s="5"/>
       <c r="Y8" s="1"/>
-      <c r="AH8" s="1"/>
+      <c r="AA8" s="1" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J9" s="1"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="5"/>
       <c r="Y9" s="1"/>
-      <c r="AH9" s="1"/>
+      <c r="AA9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J10" s="1"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="5"/>
       <c r="Y10" s="1"/>
-      <c r="AH10" s="1"/>
+      <c r="AA10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J11" s="1"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="5"/>
       <c r="Y11" s="1"/>
-      <c r="AH11" s="1"/>
+      <c r="AA11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J12" s="1"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="5"/>
+      <c r="S12" s="16" t="str" cm="1">
+        <f t="array" ref="S12">_xlfn.SWITCH(E3,"WI","","IA","","IL","","MI","","MO","","NE","","STATES MUST BE IA, IL, MI, MO, NE, OR WI")</f>
+        <v/>
+      </c>
       <c r="Y12" s="1"/>
-      <c r="AH12" s="1"/>
+      <c r="AA12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J13" s="1"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="5"/>
       <c r="Y13" s="1"/>
-      <c r="AH13" s="1"/>
+      <c r="AA13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J14" s="1"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="5"/>
       <c r="Y14" s="1"/>
-      <c r="AH14" s="1"/>
+      <c r="AA14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J15" s="1"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="5"/>
       <c r="Y15" s="1"/>
-      <c r="AH15" s="1"/>
+      <c r="AA15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J16" s="1"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="5"/>
       <c r="Y16" s="1"/>
-      <c r="AH16" s="1"/>
+      <c r="AA16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
     <row r="17" spans="10:36" x14ac:dyDescent="0.25">
       <c r="J17" s="1"/>
-      <c r="K17" s="10"/>
+      <c r="K17" s="5"/>
       <c r="Y17" s="1"/>
-      <c r="AH17" s="1"/>
+      <c r="AA17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
     <row r="18" spans="10:36" x14ac:dyDescent="0.25">
       <c r="J18" s="1"/>
-      <c r="K18" s="10"/>
+      <c r="K18" s="5"/>
+      <c r="U18" t="str" cm="1">
+        <f t="array" ref="U18:U23">IF(ISBLANK(A3),"LAST NAME REQUIRED",IF(ISBLANK(B3),"FIRST NAME REQUIRED",IF(ISBLANK(C3),"ADDRESS REQUIRED",IF(ISBLANK(D3),"CITY REQUIRED",IF(NOT(E3=VAL_STATES),"STATES MUST BE IA, IL, MI, MO, NE, OR WI","FALSE")))))</f>
+        <v>FALSE</v>
+      </c>
       <c r="Y18" s="1"/>
-      <c r="AH18" s="1"/>
+      <c r="AA18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
     <row r="19" spans="10:36" x14ac:dyDescent="0.25">
       <c r="J19" s="1"/>
-      <c r="K19" s="10"/>
+      <c r="K19" s="5"/>
+      <c r="U19" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
       <c r="Y19" s="1"/>
-      <c r="AH19" s="1"/>
+      <c r="AA19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
     <row r="20" spans="10:36" x14ac:dyDescent="0.25">
       <c r="J20" s="1"/>
-      <c r="K20" s="10"/>
-      <c r="Z20" s="7"/>
-      <c r="AH20" s="1"/>
+      <c r="K20" s="5"/>
+      <c r="U20" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="4"/>
       <c r="AJ20" s="1"/>
+    </row>
+    <row r="21" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="U21" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
+    </row>
+    <row r="22" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="U22" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
+    </row>
+    <row r="23" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="U23" t="str">
+        <v>STATES MUST BE IA, IL, MI, MO, NE, OR WI</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="L1:Y1"/>
-    <mergeCell ref="Z1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>